<commit_message>
Revisions to form definitions for parent-child forms. NOTE -- formDef.json needed to be hand-editted.
</commit_message>
<xml_diff>
--- a/form-files/household/household.xlsx
+++ b/form-files/household/household.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-10716" yWindow="300" windowWidth="23652" windowHeight="18240" activeTab="2"/>
+    <workbookView xWindow="-10716" yWindow="300" windowWidth="23652" windowHeight="18240"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="3" r:id="rId2"/>
     <sheet name="settings" sheetId="4" r:id="rId3"/>
+    <sheet name="model" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>type</t>
   </si>
@@ -118,13 +119,131 @@
   </si>
   <si>
     <t>household</t>
+  </si>
+  <si>
+    <t>table_id</t>
+  </si>
+  <si>
+    <t>household_member</t>
+  </si>
+  <si>
+    <t>line_subtext.elementName</t>
+  </si>
+  <si>
+    <t>line_subtext.isInstanceMetadata</t>
+  </si>
+  <si>
+    <t>line_text.isInstanceMetadata</t>
+  </si>
+  <si>
+    <t>line_text.elementName</t>
+  </si>
+  <si>
+    <t>instanceName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">listing of subforms displays the line_text in larger font, and the line_subtext in smaller font beside an 'edit' button. </t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>household_id</t>
+  </si>
+  <si>
+    <t>Unique barcode ID or locator designation for this household</t>
+  </si>
+  <si>
+    <t>schema.type</t>
+  </si>
+  <si>
+    <t>schema.joins[0].table_id</t>
+  </si>
+  <si>
+    <t>schema.joins[0].element_name</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This would insert a 'joins' entry into the column_definitions table for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>household_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> column of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>household</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> table_id of the form: 
+"[ { table_id: household_member, element_name: household_id } ]"
+The way to define joins is undoubtedly broken in the current XLSXConverter, as there is no way to parse lists of values (as far as I know). I will research how to fix this.</t>
+    </r>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>joined_through_name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>joined_through_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> value identifies the name (elementName) in the model that should be used when scanning in the joins lists for the table_id to discover the foreign key column to filter on in the subform.
+If this is omitted, we would probably just scan the entire model to see if table_id appears anywhere and use the first match we find. </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -141,6 +260,13 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -167,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -180,6 +306,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,21 +611,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" customWidth="1"/>
-    <col min="4" max="4" width="40" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" customWidth="1"/>
+    <col min="4" max="4" width="38" customWidth="1"/>
+    <col min="5" max="6" width="20.21875" customWidth="1"/>
+    <col min="7" max="7" width="31.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" customWidth="1"/>
+    <col min="9" max="9" width="27.77734375" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
+    <col min="11" max="11" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,73 +644,130 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:11" ht="169.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -658,10 +851,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -701,6 +894,74 @@
         <v>32</v>
       </c>
     </row>
+    <row r="5" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="192.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:5" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>